<commit_message>
Added initial rows to MAIN table
Rows resulted from Data_Summary_Pharm_Haz_Parenteral_Prep 10.6.21
</commit_message>
<xml_diff>
--- a/P3OME_MAIN_TABLE.xlsx
+++ b/P3OME_MAIN_TABLE.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajf/Desktop/BASKET/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajf/Documents/GitHub/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15163D61-74CB-EE4A-BC1A-B981111BFB8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A44F1C4-3D33-9C4D-87CA-CE964C88472E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-600" yWindow="-18880" windowWidth="30860" windowHeight="17040" xr2:uid="{BF91EB68-8200-D04C-ACEA-7728D8B81486}"/>
+    <workbookView xWindow="-4140" yWindow="-19220" windowWidth="30860" windowHeight="17040" xr2:uid="{BF91EB68-8200-D04C-ACEA-7728D8B81486}"/>
   </bookViews>
   <sheets>
     <sheet name="P3ome" sheetId="1" r:id="rId1"/>
     <sheet name="P3ome Terms" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="88">
   <si>
     <t>Final Pharmacy Product Type</t>
   </si>
@@ -107,9 +107,6 @@
   </si>
   <si>
     <t>P3OME Identifier</t>
-  </si>
-  <si>
-    <t>PURPOSES FOR TOUCHES</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -188,12 +185,186 @@
   <si>
     <t>P3ome Identifer</t>
   </si>
+  <si>
+    <t xml:space="preserve">Hazardous Pharmacy-Provided Packaging </t>
+  </si>
+  <si>
+    <t>Pharmacy Process Stage</t>
+  </si>
+  <si>
+    <t>Preparation</t>
+  </si>
+  <si>
+    <t>Enteral</t>
+  </si>
+  <si>
+    <t>Parenteral</t>
+  </si>
+  <si>
+    <t>Hazardous</t>
+  </si>
+  <si>
+    <t>Patient-specific</t>
+  </si>
+  <si>
+    <t>Syringe</t>
+  </si>
+  <si>
+    <t>IV bag</t>
+  </si>
+  <si>
+    <t>CSTD used</t>
+  </si>
+  <si>
+    <t>Closed System Drug-Transfer Device</t>
+  </si>
+  <si>
+    <t>Add and fill IV line</t>
+  </si>
+  <si>
+    <t>TOUCHES BY PURPOSE</t>
+  </si>
+  <si>
+    <t>Remove from Storage</t>
+  </si>
+  <si>
+    <t>Scan before Sterile Compouding</t>
+  </si>
+  <si>
+    <t>Connect CTSD</t>
+  </si>
+  <si>
+    <t>Reconstitute</t>
+  </si>
+  <si>
+    <t>Remove Drug Solution from Vial into Syringe</t>
+  </si>
+  <si>
+    <t>Inject Drug Solution into IV Bag</t>
+  </si>
+  <si>
+    <t>Weigh Compounded Drug Product</t>
+  </si>
+  <si>
+    <t>Reconstitution Required</t>
+  </si>
+  <si>
+    <t>Affix Label and Place in Hazardous Delivery Bag</t>
+  </si>
+  <si>
+    <t>Filled and Labeled IV Bag in Hazard Delivery Bag</t>
+  </si>
+  <si>
+    <t>Filled and Labeled Injectable Syringe in Hazard Delivery Bag</t>
+  </si>
+  <si>
+    <t>Attached IV line required</t>
+  </si>
+  <si>
+    <t>Product Identifer</t>
+  </si>
+  <si>
+    <t>e84153ae-9c2a-4f98-83f7-e5a3c8d15403</t>
+  </si>
+  <si>
+    <t>cc496dc0-b4e6-46a8-869d-50fce3c5d694</t>
+  </si>
+  <si>
+    <t>85663ebc-92d5-40bf-bbb1-4ab5ac7aab62</t>
+  </si>
+  <si>
+    <t>0d303436-fb61-458d-9c3b-3e18c439cb3e</t>
+  </si>
+  <si>
+    <t>b4c2fa64-23dd-434b-99b8-76142d2098ad</t>
+  </si>
+  <si>
+    <t>89cf804e-740a-440c-85d2-034173ecacef</t>
+  </si>
+  <si>
+    <t>dacc1a93-0c4b-451a-9e5a-bec7726766cc</t>
+  </si>
+  <si>
+    <t>d9bbc29f-f7cc-4aa1-a02b-33c0a79e5a8e</t>
+  </si>
+  <si>
+    <t>cf9a7f7d-39fd-4d8f-b0d8-954d361d3119</t>
+  </si>
+  <si>
+    <t>88b9ccb7-052f-4c7b-9602-e531231076e0</t>
+  </si>
+  <si>
+    <t>f33a045a-13b4-4238-82c9-622f86b5ac04</t>
+  </si>
+  <si>
+    <t>fa2d7dc1-858a-4d63-a449-ed83fcc0c494</t>
+  </si>
+  <si>
+    <t>127ff706-5237-43d3-a2e1-b00bf54281d3</t>
+  </si>
+  <si>
+    <t>28d9bd75-c0e4-46b1-9288-891c585067de</t>
+  </si>
+  <si>
+    <t>284ef53d-2741-4e69-9752-6c7055c90a9f</t>
+  </si>
+  <si>
+    <t>7e5d592f-3656-4c99-a95c-586440c4b5e1</t>
+  </si>
+  <si>
+    <t>8b74b937-87f4-418c-a75a-6d7ac1741d46</t>
+  </si>
+  <si>
+    <t>3e4389ec-a72a-42e7-827e-667c9053e548</t>
+  </si>
+  <si>
+    <t>826a48bd-cabb-466c-8585-44606450cb32</t>
+  </si>
+  <si>
+    <t>b00b0f23-cfdf-4d8e-8db5-b0a6a262c981</t>
+  </si>
+  <si>
+    <t>4ff655ee-8256-4267-b7d5-8d575884bf55</t>
+  </si>
+  <si>
+    <t>c1745cd6-aa9f-4cc3-9303-d120c77d577f</t>
+  </si>
+  <si>
+    <t>ae83e1ce-ce35-4382-9ea2-28f41c83d5f9</t>
+  </si>
+  <si>
+    <t>11685f29-2ccb-46ee-82b5-01978d26d02d</t>
+  </si>
+  <si>
+    <t>65d5f241-b153-472b-8c27-efa7a85c875f</t>
+  </si>
+  <si>
+    <t>1869ada3-8eca-4aa1-9ed3-c4935bfa663b</t>
+  </si>
+  <si>
+    <t>39875e84-7485-4f84-9713-62823abdda1d</t>
+  </si>
+  <si>
+    <t>9d6ecc87-fa1a-48d6-ae08-c6c418edc8c9</t>
+  </si>
+  <si>
+    <t>6ea86ed6-5660-46e1-8774-75535120b57a</t>
+  </si>
+  <si>
+    <t>5e6cbb43-68f0-4192-a7e5-dc1e04a08413</t>
+  </si>
+  <si>
+    <t>FLISHDB</t>
+  </si>
+  <si>
+    <t>FLIVPBHDB</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -285,6 +456,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -342,7 +520,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -426,17 +604,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -445,18 +641,29 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -472,21 +679,48 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -801,324 +1035,1224 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{470AE0E9-15FB-9B45-982A-B5C4188457EE}">
-  <dimension ref="A1:AQ22"/>
+  <dimension ref="A1:AS33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AK9" sqref="AK9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="1"/>
-    <col min="3" max="3" width="30" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="35.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="62.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="41.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="42.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.83203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" style="1" customWidth="1"/>
+    <col min="14" max="17" width="10.83203125" style="1"/>
+    <col min="18" max="18" width="13" style="1" customWidth="1"/>
+    <col min="19" max="19" width="26.5" style="1" customWidth="1"/>
+    <col min="20" max="20" width="28.6640625" style="1" customWidth="1"/>
+    <col min="21" max="23" width="10.83203125" style="1"/>
+    <col min="24" max="24" width="23.1640625" style="1" customWidth="1"/>
+    <col min="25" max="25" width="35.5" style="1" customWidth="1"/>
+    <col min="26" max="26" width="19.5" style="1" customWidth="1"/>
+    <col min="27" max="27" width="19.6640625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="44.6640625" style="1" customWidth="1"/>
+    <col min="29" max="29" width="35.83203125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="40.1640625" style="1" customWidth="1"/>
+    <col min="31" max="31" width="29" style="1" customWidth="1"/>
+    <col min="32" max="32" width="49.5" style="1" customWidth="1"/>
+    <col min="33" max="33" width="39.33203125" style="1" customWidth="1"/>
+    <col min="34" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:45" ht="95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="22"/>
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="22"/>
+      <c r="AG1" s="22"/>
+      <c r="AH1" s="22"/>
+      <c r="AI1" s="22"/>
+      <c r="AJ1" s="22"/>
+      <c r="AK1" s="22"/>
+      <c r="AL1" s="22"/>
+      <c r="AM1" s="22"/>
+      <c r="AN1" s="22"/>
+      <c r="AO1" s="22"/>
+      <c r="AP1" s="22"/>
+      <c r="AQ1" s="22"/>
+      <c r="AR1" s="22"/>
+      <c r="AS1" s="22"/>
+    </row>
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="16"/>
+      <c r="I2" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
+      <c r="X2" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="15"/>
+      <c r="AA2" s="15"/>
+      <c r="AB2" s="15"/>
+      <c r="AC2" s="15"/>
+      <c r="AD2" s="15"/>
+      <c r="AE2" s="15"/>
+      <c r="AF2" s="15"/>
+      <c r="AG2" s="15"/>
+      <c r="AH2" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="3"/>
-      <c r="AC1" s="3"/>
-      <c r="AD1" s="3"/>
-      <c r="AE1" s="3"/>
-      <c r="AF1" s="3"/>
-      <c r="AG1" s="3"/>
-      <c r="AH1" s="3"/>
-      <c r="AI1" s="3"/>
-      <c r="AJ1" s="3"/>
-      <c r="AK1" s="3"/>
-      <c r="AL1" s="3"/>
-      <c r="AM1" s="3"/>
-      <c r="AN1" s="3"/>
-      <c r="AO1" s="3"/>
-      <c r="AP1" s="3"/>
-      <c r="AQ1" s="3"/>
-    </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="15" t="s">
+      <c r="AI2" s="14"/>
+      <c r="AJ2" s="14"/>
+      <c r="AK2" s="14"/>
+      <c r="AL2" s="14"/>
+      <c r="AM2" s="14"/>
+      <c r="AN2" s="14"/>
+      <c r="AO2" s="14"/>
+      <c r="AP2" s="14"/>
+      <c r="AQ2" s="14"/>
+      <c r="AR2" s="14"/>
+      <c r="AS2" s="14"/>
+    </row>
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A3" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="33"/>
+      <c r="P3" s="33"/>
+      <c r="Q3" s="33"/>
+      <c r="R3" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="S3" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="T3" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="U3" s="33"/>
+      <c r="V3" s="33"/>
+      <c r="W3" s="33"/>
+      <c r="X3" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y3" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z3" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA3" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB3" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC3" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD3" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE3" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF3" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG3" s="35"/>
+      <c r="AH3" s="34"/>
+      <c r="AI3" s="34"/>
+      <c r="AJ3" s="34"/>
+      <c r="AK3" s="34"/>
+      <c r="AL3" s="34"/>
+      <c r="AM3" s="34"/>
+      <c r="AN3" s="34"/>
+      <c r="AO3" s="34"/>
+      <c r="AP3" s="34"/>
+      <c r="AQ3" s="34"/>
+      <c r="AR3" s="34"/>
+      <c r="AS3" s="34"/>
+    </row>
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="9">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="29">
+        <f>SUM(X4:AG4)</f>
+        <v>5</v>
+      </c>
+      <c r="H4" s="30"/>
+      <c r="I4" s="21">
+        <v>1</v>
+      </c>
+      <c r="J4" s="21">
+        <v>0</v>
+      </c>
+      <c r="K4" s="21">
+        <v>1</v>
+      </c>
+      <c r="L4" s="21">
+        <v>1</v>
+      </c>
+      <c r="M4" s="21">
+        <v>1</v>
+      </c>
+      <c r="N4" s="21">
+        <v>0</v>
+      </c>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="21">
+        <v>0</v>
+      </c>
+      <c r="S4" s="21">
+        <v>0</v>
+      </c>
+      <c r="T4" s="21">
+        <v>0</v>
+      </c>
+      <c r="U4" s="21"/>
+      <c r="V4" s="21"/>
+      <c r="W4" s="21"/>
+      <c r="X4" s="21">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="21">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="21">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="21">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="21">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="21">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="21">
+        <v>1</v>
+      </c>
+      <c r="AE4" s="21">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="21">
+        <v>1</v>
+      </c>
+      <c r="AG4" s="21"/>
+      <c r="AH4" s="21"/>
+      <c r="AI4" s="21"/>
+      <c r="AJ4" s="21"/>
+      <c r="AK4" s="21"/>
+      <c r="AL4" s="21"/>
+      <c r="AM4" s="21"/>
+      <c r="AN4" s="21"/>
+      <c r="AO4" s="21"/>
+      <c r="AP4" s="21"/>
+      <c r="AQ4" s="21"/>
+      <c r="AR4" s="21"/>
+      <c r="AS4" s="21"/>
+    </row>
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="9">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="24">
+        <f>SUM(X5:AG5)</f>
+        <v>6</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="21">
+        <v>1</v>
+      </c>
+      <c r="J5" s="21">
+        <v>0</v>
+      </c>
+      <c r="K5" s="21">
+        <v>1</v>
+      </c>
+      <c r="L5" s="21">
+        <v>1</v>
+      </c>
+      <c r="M5" s="21">
+        <v>0</v>
+      </c>
+      <c r="N5" s="21">
+        <v>1</v>
+      </c>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21">
+        <v>0</v>
+      </c>
+      <c r="S5" s="21">
+        <v>0</v>
+      </c>
+      <c r="T5" s="21">
+        <v>0</v>
+      </c>
+      <c r="U5" s="21"/>
+      <c r="V5" s="21"/>
+      <c r="W5" s="21"/>
+      <c r="X5" s="21">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="21">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="21">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="21">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="21">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="21">
+        <v>1</v>
+      </c>
+      <c r="AD5" s="21">
+        <v>1</v>
+      </c>
+      <c r="AE5" s="21">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="21">
+        <v>1</v>
+      </c>
+      <c r="AG5" s="21"/>
+      <c r="AH5" s="21"/>
+      <c r="AI5" s="21"/>
+      <c r="AJ5" s="21"/>
+      <c r="AK5" s="21"/>
+      <c r="AL5" s="21"/>
+      <c r="AM5" s="21"/>
+      <c r="AN5" s="21"/>
+      <c r="AO5" s="21"/>
+      <c r="AP5" s="21"/>
+      <c r="AQ5" s="21"/>
+      <c r="AR5" s="21"/>
+      <c r="AS5" s="21"/>
+    </row>
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="9">
         <v>3</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="17" t="s">
+      <c r="D6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="24">
+        <f>SUM(X6:AG6)</f>
+        <v>6</v>
+      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="21">
+        <v>1</v>
+      </c>
+      <c r="J6" s="21">
+        <v>0</v>
+      </c>
+      <c r="K6" s="21">
+        <v>1</v>
+      </c>
+      <c r="L6" s="21">
+        <v>1</v>
+      </c>
+      <c r="M6" s="21">
+        <v>1</v>
+      </c>
+      <c r="N6" s="21">
+        <v>0</v>
+      </c>
+      <c r="O6" s="21"/>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="21"/>
+      <c r="R6" s="21">
+        <v>1</v>
+      </c>
+      <c r="S6" s="21">
+        <v>0</v>
+      </c>
+      <c r="T6" s="21">
+        <v>0</v>
+      </c>
+      <c r="U6" s="21"/>
+      <c r="V6" s="21"/>
+      <c r="W6" s="21"/>
+      <c r="X6" s="21">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="21">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="21">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="21">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="21">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="21">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="21">
+        <v>1</v>
+      </c>
+      <c r="AE6" s="21">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="21">
+        <v>1</v>
+      </c>
+      <c r="AG6" s="21"/>
+      <c r="AH6" s="21"/>
+      <c r="AI6" s="21"/>
+      <c r="AJ6" s="21"/>
+      <c r="AK6" s="21"/>
+      <c r="AL6" s="21"/>
+      <c r="AM6" s="21"/>
+      <c r="AN6" s="21"/>
+      <c r="AO6" s="21"/>
+      <c r="AP6" s="21"/>
+      <c r="AQ6" s="21"/>
+      <c r="AR6" s="21"/>
+      <c r="AS6" s="21"/>
+    </row>
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="9">
         <v>4</v>
       </c>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="18" t="s">
+      <c r="D7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="24">
+        <f>SUM(X7:AG7)</f>
+        <v>7</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="21">
+        <v>1</v>
+      </c>
+      <c r="J7" s="21">
+        <v>0</v>
+      </c>
+      <c r="K7" s="21">
+        <v>1</v>
+      </c>
+      <c r="L7" s="21">
+        <v>1</v>
+      </c>
+      <c r="M7" s="21">
+        <v>0</v>
+      </c>
+      <c r="N7" s="21">
+        <v>1</v>
+      </c>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="21">
+        <v>1</v>
+      </c>
+      <c r="S7" s="21">
+        <v>0</v>
+      </c>
+      <c r="T7" s="21">
+        <v>0</v>
+      </c>
+      <c r="U7" s="21"/>
+      <c r="V7" s="21"/>
+      <c r="W7" s="21"/>
+      <c r="X7" s="21">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="21">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="21">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="21">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="21">
+        <v>1</v>
+      </c>
+      <c r="AC7" s="21">
+        <v>1</v>
+      </c>
+      <c r="AD7" s="21">
+        <v>1</v>
+      </c>
+      <c r="AE7" s="21">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="21">
+        <v>1</v>
+      </c>
+      <c r="AG7" s="21"/>
+      <c r="AH7" s="21"/>
+      <c r="AI7" s="21"/>
+      <c r="AJ7" s="21"/>
+      <c r="AK7" s="21"/>
+      <c r="AL7" s="21"/>
+      <c r="AM7" s="21"/>
+      <c r="AN7" s="21"/>
+      <c r="AO7" s="21"/>
+      <c r="AP7" s="21"/>
+      <c r="AQ7" s="21"/>
+      <c r="AR7" s="21"/>
+      <c r="AS7" s="21"/>
+    </row>
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="9">
         <v>5</v>
       </c>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="18"/>
-      <c r="U2" s="18"/>
-      <c r="V2" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="W2" s="14"/>
-      <c r="X2" s="14"/>
-      <c r="Y2" s="14"/>
-      <c r="Z2" s="14"/>
-      <c r="AA2" s="14"/>
-      <c r="AB2" s="14"/>
-      <c r="AC2" s="14"/>
-      <c r="AD2" s="14"/>
-      <c r="AE2" s="14"/>
-      <c r="AF2" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="AG2" s="23"/>
-      <c r="AH2" s="23"/>
-      <c r="AI2" s="23"/>
-      <c r="AJ2" s="23"/>
-      <c r="AK2" s="23"/>
-      <c r="AL2" s="23"/>
-      <c r="AM2" s="23"/>
-      <c r="AN2" s="23"/>
-      <c r="AO2" s="23"/>
-      <c r="AP2" s="23"/>
-      <c r="AQ2" s="23"/>
-    </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="11" t="s">
+      <c r="D8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="24">
+        <f t="shared" ref="G8:G11" si="0">SUM(X8:AG8)</f>
+        <v>7</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="21">
+        <v>1</v>
+      </c>
+      <c r="J8" s="21">
+        <v>0</v>
+      </c>
+      <c r="K8" s="21">
+        <v>1</v>
+      </c>
+      <c r="L8" s="21">
+        <v>1</v>
+      </c>
+      <c r="M8" s="21">
+        <v>1</v>
+      </c>
+      <c r="N8" s="21">
+        <v>0</v>
+      </c>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="21">
+        <v>1</v>
+      </c>
+      <c r="S8" s="21">
+        <v>1</v>
+      </c>
+      <c r="T8" s="21">
+        <v>0</v>
+      </c>
+      <c r="U8" s="21"/>
+      <c r="V8" s="21"/>
+      <c r="W8" s="21"/>
+      <c r="X8" s="21">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="21">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="21">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="21">
+        <v>1</v>
+      </c>
+      <c r="AB8" s="21">
+        <v>1</v>
+      </c>
+      <c r="AC8" s="21">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="21">
+        <v>1</v>
+      </c>
+      <c r="AE8" s="21">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="21">
+        <v>1</v>
+      </c>
+      <c r="AG8" s="21"/>
+      <c r="AH8" s="21"/>
+      <c r="AI8" s="21"/>
+      <c r="AJ8" s="21"/>
+      <c r="AK8" s="21"/>
+      <c r="AL8" s="21"/>
+      <c r="AM8" s="21"/>
+      <c r="AN8" s="21"/>
+      <c r="AO8" s="21"/>
+      <c r="AP8" s="21"/>
+      <c r="AQ8" s="21"/>
+      <c r="AR8" s="21"/>
+      <c r="AS8" s="21"/>
+    </row>
+    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="9">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="D9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="24">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="21">
+        <v>1</v>
+      </c>
+      <c r="J9" s="21">
+        <v>0</v>
+      </c>
+      <c r="K9" s="21">
+        <v>1</v>
+      </c>
+      <c r="L9" s="21">
+        <v>1</v>
+      </c>
+      <c r="M9" s="21">
+        <v>0</v>
+      </c>
+      <c r="N9" s="21">
+        <v>1</v>
+      </c>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="21"/>
+      <c r="R9" s="21">
+        <v>1</v>
+      </c>
+      <c r="S9" s="21">
+        <v>1</v>
+      </c>
+      <c r="T9" s="21">
+        <v>0</v>
+      </c>
+      <c r="U9" s="21"/>
+      <c r="V9" s="21"/>
+      <c r="W9" s="21"/>
+      <c r="X9" s="21">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="21">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="21">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="21">
+        <v>1</v>
+      </c>
+      <c r="AB9" s="21">
+        <v>1</v>
+      </c>
+      <c r="AC9" s="21">
+        <v>1</v>
+      </c>
+      <c r="AD9" s="21">
+        <v>1</v>
+      </c>
+      <c r="AE9" s="21">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="21">
+        <v>1</v>
+      </c>
+      <c r="AG9" s="21"/>
+      <c r="AH9" s="21"/>
+      <c r="AI9" s="21"/>
+      <c r="AJ9" s="21"/>
+      <c r="AK9" s="21"/>
+      <c r="AL9" s="21"/>
+      <c r="AM9" s="21"/>
+      <c r="AN9" s="21"/>
+      <c r="AO9" s="21"/>
+      <c r="AP9" s="21"/>
+      <c r="AQ9" s="21"/>
+      <c r="AR9" s="21"/>
+      <c r="AS9" s="21"/>
+    </row>
+    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="9">
         <v>7</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="D10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="24">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-    </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13">
-        <v>1</v>
-      </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-    </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13">
-        <v>2</v>
-      </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-    </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="13">
-        <v>3</v>
-      </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-    </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13">
-        <v>4</v>
-      </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-    </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13">
-        <v>5</v>
-      </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-    </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13">
-        <v>6</v>
-      </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-    </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13">
-        <v>7</v>
-      </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-    </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13">
+      <c r="H10" s="6"/>
+      <c r="I10" s="21">
+        <v>1</v>
+      </c>
+      <c r="J10" s="21">
+        <v>0</v>
+      </c>
+      <c r="K10" s="21">
+        <v>1</v>
+      </c>
+      <c r="L10" s="21">
+        <v>1</v>
+      </c>
+      <c r="M10" s="21">
+        <v>1</v>
+      </c>
+      <c r="N10" s="21">
+        <v>0</v>
+      </c>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="21"/>
+      <c r="R10" s="21">
+        <v>1</v>
+      </c>
+      <c r="S10" s="21">
+        <v>1</v>
+      </c>
+      <c r="T10" s="21">
+        <v>1</v>
+      </c>
+      <c r="U10" s="21"/>
+      <c r="V10" s="21"/>
+      <c r="W10" s="21"/>
+      <c r="X10" s="21">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="21">
+        <v>1</v>
+      </c>
+      <c r="Z10" s="21">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="21">
+        <v>1</v>
+      </c>
+      <c r="AB10" s="21">
+        <v>1</v>
+      </c>
+      <c r="AC10" s="21">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="21">
+        <v>1</v>
+      </c>
+      <c r="AE10" s="21">
+        <v>1</v>
+      </c>
+      <c r="AF10" s="21">
+        <v>1</v>
+      </c>
+      <c r="AG10" s="21"/>
+      <c r="AH10" s="21"/>
+      <c r="AI10" s="21"/>
+      <c r="AJ10" s="21"/>
+      <c r="AK10" s="21"/>
+      <c r="AL10" s="21"/>
+      <c r="AM10" s="21"/>
+      <c r="AN10" s="21"/>
+      <c r="AO10" s="21"/>
+      <c r="AP10" s="21"/>
+      <c r="AQ10" s="21"/>
+      <c r="AR10" s="21"/>
+      <c r="AS10" s="21"/>
+    </row>
+    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="9">
         <v>8</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-    </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13">
+      <c r="D11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="24">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-    </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13">
+      <c r="H11" s="6"/>
+      <c r="I11" s="21">
+        <v>1</v>
+      </c>
+      <c r="J11" s="21">
+        <v>0</v>
+      </c>
+      <c r="K11" s="21">
+        <v>1</v>
+      </c>
+      <c r="L11" s="21">
+        <v>1</v>
+      </c>
+      <c r="M11" s="21">
+        <v>0</v>
+      </c>
+      <c r="N11" s="21">
+        <v>1</v>
+      </c>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="21"/>
+      <c r="R11" s="21">
+        <v>1</v>
+      </c>
+      <c r="S11" s="21">
+        <v>1</v>
+      </c>
+      <c r="T11" s="21">
+        <v>1</v>
+      </c>
+      <c r="U11" s="21"/>
+      <c r="V11" s="21"/>
+      <c r="W11" s="21"/>
+      <c r="X11" s="21">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="21">
+        <v>1</v>
+      </c>
+      <c r="Z11" s="21">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="21">
+        <v>1</v>
+      </c>
+      <c r="AB11" s="21">
+        <v>1</v>
+      </c>
+      <c r="AC11" s="21">
+        <v>1</v>
+      </c>
+      <c r="AD11" s="21">
+        <v>1</v>
+      </c>
+      <c r="AE11" s="21">
+        <v>1</v>
+      </c>
+      <c r="AF11" s="21">
+        <v>1</v>
+      </c>
+      <c r="AG11" s="21"/>
+      <c r="AH11" s="21"/>
+      <c r="AI11" s="21"/>
+      <c r="AJ11" s="21"/>
+      <c r="AK11" s="21"/>
+      <c r="AL11" s="21"/>
+      <c r="AM11" s="21"/>
+      <c r="AN11" s="21"/>
+      <c r="AO11" s="21"/>
+      <c r="AP11" s="21"/>
+      <c r="AQ11" s="21"/>
+      <c r="AR11" s="21"/>
+      <c r="AS11" s="21"/>
+    </row>
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A12" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9">
+        <v>9</v>
+      </c>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A13" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9">
         <v>10</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-    </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13">
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A14" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9">
         <v>11</v>
       </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-    </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13">
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A15" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9">
         <v>12</v>
       </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-    </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13">
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A16" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="9">
         <v>13</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="13">
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="9">
         <v>14</v>
       </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="13">
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="9">
         <v>15</v>
       </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="13">
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="9">
         <v>16</v>
       </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="13">
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="9">
         <v>17</v>
       </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="13">
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="9">
         <v>18</v>
       </c>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="13">
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="9">
         <v>19</v>
       </c>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="28" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="28" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="27" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="27" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="27" t="s">
+        <v>85</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="AF2:AQ2"/>
-    <mergeCell ref="V2:AE2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="G2:O2"/>
-    <mergeCell ref="P2:U2"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="AH2:AS2"/>
+    <mergeCell ref="X2:AG2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="I2:Q2"/>
+    <mergeCell ref="R2:W2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1134,37 +2268,37 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.1640625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="27.1640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="32.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="97.5" style="4" customWidth="1"/>
-    <col min="4" max="4" width="32.6640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="54.5" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="4"/>
+    <col min="3" max="3" width="97.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="54.5" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1240,7 +2374,7 @@
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1249,7 +2383,7 @@
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>

</xml_diff>